<commit_message>
Updated IND model - 2025-08-07 09:00
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3636AA54-AFC6-4409-8BB6-D8D08977497C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05880BF2-6DBA-48AE-9432-A685D8E5A485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S3aH2,S3b0330h07,S3b0330h17,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S1aH6,S3b0330h11,S6d1221h11,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3b0330h14,S6aH7,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S6d1221h08,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3b0330h13,S6aH5,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S4aH2,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3aH3,S3b0330h15,S6d1221h13,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15</t>
-  </si>
-  <si>
-    <t>S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S4aH1,S4c0615h04,S6aH1,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h20,S4c0615h01,S6d1221h03,S3aH1,S4c0615h24,S6d1221h01,S3b0330h05,S4c0615h21,S6d1221h06,S1aH1,S3b0330h04,S3b0330h19,S4c0615h20,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S6d1221h21,S2aH1,S5aH8,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h06,S3b0330h21,S2aH8</t>
+    <t>S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3aH2,S3b0330h07,S3b0330h17,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH6,S3b0330h11,S6d1221h11,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S4aH2,S3aH3,S3b0330h15,S6d1221h13,S3b0330h13,S6aH5,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S6d1221h08</t>
+  </si>
+  <si>
+    <t>S3b0330h19,S4c0615h20,S3b0330h01,S3b0330h03,S4c0615h05,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S4aH1,S4c0615h04,S6aH1,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h20,S4c0615h01,S6d1221h03,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S2aH1,S5aH8,S3b0330h06,S3b0330h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S6d1221h21,S3aH1,S4c0615h24,S6d1221h01,S2aH8,S1aH1,S3b0330h04</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S4aH1,S4c0615h04,S6aH1,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h20,S4c0615h01,S6d1221h03,S3aH1,S4c0615h24,S6d1221h01,S3b0330h05,S4c0615h21,S6d1221h06,S1aH1,S3b0330h04,S3b0330h19,S4c0615h20,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S6d1221h21,S2aH1,S5aH8,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h06,S3b0330h21,S2aH8</v>
+        <v>S3b0330h19,S4c0615h20,S3b0330h01,S3b0330h03,S4c0615h05,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S4aH1,S4c0615h04,S6aH1,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h20,S4c0615h01,S6d1221h03,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S2aH1,S5aH8,S3b0330h06,S3b0330h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S6d1221h21,S3aH1,S4c0615h24,S6d1221h01,S2aH8,S1aH1,S3b0330h04</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S3aH2,S3b0330h07,S3b0330h17,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S1aH6,S3b0330h11,S6d1221h11,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3b0330h14,S6aH7,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S6d1221h08,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3b0330h13,S6aH5,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S4aH2,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3aH3,S3b0330h15,S6d1221h13,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15</v>
+        <v>S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3aH2,S3b0330h07,S3b0330h17,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH6,S3b0330h11,S6d1221h11,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S4aH2,S3aH3,S3b0330h15,S6d1221h13,S3b0330h13,S6aH5,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S6d1221h08</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E666DAE-0D15-4C38-98E6-CFEE3B005392}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E332C8FC-F448-4A77-96D4-2A7B6FEA8460}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7183C6E7-0E62-4F36-9B81-3DB33AFD0770}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3632209D-3E8B-4842-B9A1-FE29620B4596}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2945,10 +2945,10 @@
         <v>171</v>
       </c>
       <c r="M4" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="N4">
-        <v>0.64374644043026463</v>
+        <v>6.3366251517854258E-2</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="N5">
-        <v>6.1341729440462511E-2</v>
+        <v>5.6196606453970052E-2</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3015,10 +3015,10 @@
         <v>171</v>
       </c>
       <c r="M6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="N6">
-        <v>5.6196606453970059E-2</v>
+        <v>6.134172944046249E-2</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3053,7 +3053,7 @@
         <v>84</v>
       </c>
       <c r="N7">
-        <v>0.12151000977874253</v>
+        <v>0.1215100097787425</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3085,10 +3085,10 @@
         <v>171</v>
       </c>
       <c r="M8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="N8">
-        <v>6.3366251517854272E-2</v>
+        <v>0.2538389623787059</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="N9">
-        <v>0.25383896237870601</v>
+        <v>0.64374644043026452</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678BC6E8-68C9-441F-8BF5-20475E8A0517}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5AD754-736A-4A8B-A3A9-21A1F2EB07AC}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 09:10
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05880BF2-6DBA-48AE-9432-A685D8E5A485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951A6620-ADD9-4C69-8001-3284688F2B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3aH2,S3b0330h07,S3b0330h17,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH6,S3b0330h11,S6d1221h11,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S4aH2,S3aH3,S3b0330h15,S6d1221h13,S3b0330h13,S6aH5,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S6d1221h08</t>
-  </si>
-  <si>
-    <t>S3b0330h19,S4c0615h20,S3b0330h01,S3b0330h03,S4c0615h05,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S4aH1,S4c0615h04,S6aH1,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h20,S4c0615h01,S6d1221h03,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S2aH1,S5aH8,S3b0330h06,S3b0330h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S6d1221h21,S3aH1,S4c0615h24,S6d1221h01,S2aH8,S1aH1,S3b0330h04</t>
+    <t>S6d1221h08,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S4aH2,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3aH3,S3b0330h15,S6d1221h13,S3b0330h13,S6aH5,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH6,S3b0330h11,S6d1221h11,S3aH2,S3b0330h07,S3b0330h17,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3b0330h14,S6aH7</t>
+  </si>
+  <si>
+    <t>S1aH1,S3b0330h04,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4aH1,S4c0615h04,S6aH1,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3b0330h19,S4c0615h20,S2aH1,S5aH8,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h06,S3b0330h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S6d1221h21,S2aH8,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h20,S4c0615h01,S6d1221h03,S3aH1,S4c0615h24,S6d1221h01</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S3b0330h19,S4c0615h20,S3b0330h01,S3b0330h03,S4c0615h05,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S4aH1,S4c0615h04,S6aH1,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h20,S4c0615h01,S6d1221h03,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S2aH1,S5aH8,S3b0330h06,S3b0330h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S6d1221h21,S3aH1,S4c0615h24,S6d1221h01,S2aH8,S1aH1,S3b0330h04</v>
+        <v>S1aH1,S3b0330h04,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4aH1,S4c0615h04,S6aH1,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3b0330h19,S4c0615h20,S2aH1,S5aH8,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h06,S3b0330h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S6d1221h21,S2aH8,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h20,S4c0615h01,S6d1221h03,S3aH1,S4c0615h24,S6d1221h01</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3aH2,S3b0330h07,S3b0330h17,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH6,S3b0330h11,S6d1221h11,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S4aH2,S3aH3,S3b0330h15,S6d1221h13,S3b0330h13,S6aH5,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S6d1221h08</v>
+        <v>S6d1221h08,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S4aH2,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3aH3,S3b0330h15,S6d1221h13,S3b0330h13,S6aH5,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH6,S3b0330h11,S6d1221h11,S3aH2,S3b0330h07,S3b0330h17,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3b0330h14,S6aH7</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E332C8FC-F448-4A77-96D4-2A7B6FEA8460}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C77BF4B-75F7-43D0-94A7-7C574FB59713}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3632209D-3E8B-4842-B9A1-FE29620B4596}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FF0E56-2839-4F48-98B6-CCD54CC26F87}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2945,10 +2945,10 @@
         <v>171</v>
       </c>
       <c r="M4" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="N4">
-        <v>6.3366251517854258E-2</v>
+        <v>0.12151000977874252</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="N5">
-        <v>5.6196606453970052E-2</v>
+        <v>6.3366251517854258E-2</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3015,10 +3015,10 @@
         <v>171</v>
       </c>
       <c r="M6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N6">
-        <v>6.134172944046249E-2</v>
+        <v>0.25383896237870601</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3050,10 +3050,10 @@
         <v>171</v>
       </c>
       <c r="M7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="N7">
-        <v>0.1215100097787425</v>
+        <v>5.6196606453970052E-2</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3085,10 +3085,10 @@
         <v>171</v>
       </c>
       <c r="M8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N8">
-        <v>0.2538389623787059</v>
+        <v>6.1341729440462497E-2</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5AD754-736A-4A8B-A3A9-21A1F2EB07AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000D6DF5-064C-4B0B-8190-C36DF1AAADE8}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 09:23
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951A6620-ADD9-4C69-8001-3284688F2B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63116DB-65DB-4EAD-B876-8606EC3A4D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S6d1221h08,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S4aH2,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3aH3,S3b0330h15,S6d1221h13,S3b0330h13,S6aH5,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH6,S3b0330h11,S6d1221h11,S3aH2,S3b0330h07,S3b0330h17,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3b0330h14,S6aH7</t>
-  </si>
-  <si>
-    <t>S1aH1,S3b0330h04,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4aH1,S4c0615h04,S6aH1,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3b0330h19,S4c0615h20,S2aH1,S5aH8,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h06,S3b0330h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S6d1221h21,S2aH8,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h20,S4c0615h01,S6d1221h03,S3aH1,S4c0615h24,S6d1221h01</t>
+    <t>S4aH2,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S1aH6,S3b0330h11,S6d1221h11,S3b0330h13,S6aH5,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S6d1221h08,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH2,S3b0330h07,S3b0330h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3aH3,S3b0330h15,S6d1221h13</t>
+  </si>
+  <si>
+    <t>S2aH1,S5aH8,S3aH1,S4c0615h24,S6d1221h01,S2aH8,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S1aH1,S3b0330h04,S3b0330h01,S3b0330h03,S4c0615h05,S4aH1,S4c0615h04,S6aH1,S6d1221h21,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h20,S4c0615h01,S6d1221h03,S3b0330h19,S4c0615h20,S3b0330h06,S3b0330h21</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S1aH1,S3b0330h04,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4aH1,S4c0615h04,S6aH1,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3b0330h19,S4c0615h20,S2aH1,S5aH8,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h06,S3b0330h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S6d1221h21,S2aH8,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h20,S4c0615h01,S6d1221h03,S3aH1,S4c0615h24,S6d1221h01</v>
+        <v>S2aH1,S5aH8,S3aH1,S4c0615h24,S6d1221h01,S2aH8,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S1aH1,S3b0330h04,S3b0330h01,S3b0330h03,S4c0615h05,S4aH1,S4c0615h04,S6aH1,S6d1221h21,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h20,S4c0615h01,S6d1221h03,S3b0330h19,S4c0615h20,S3b0330h06,S3b0330h21</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S6d1221h08,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S4aH2,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3aH3,S3b0330h15,S6d1221h13,S3b0330h13,S6aH5,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH6,S3b0330h11,S6d1221h11,S3aH2,S3b0330h07,S3b0330h17,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3b0330h14,S6aH7</v>
+        <v>S4aH2,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S1aH6,S3b0330h11,S6d1221h11,S3b0330h13,S6aH5,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S6d1221h08,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH2,S3b0330h07,S3b0330h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3aH3,S3b0330h15,S6d1221h13</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C77BF4B-75F7-43D0-94A7-7C574FB59713}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FF797E-EDA3-4AE5-B67D-71DAE26DAA37}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FF0E56-2839-4F48-98B6-CCD54CC26F87}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBD3115-5910-403B-A207-72C1AC0F67F9}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2945,10 +2945,10 @@
         <v>171</v>
       </c>
       <c r="M4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="N4">
-        <v>0.12151000977874252</v>
+        <v>0.64374644043026452</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -3015,10 +3015,10 @@
         <v>171</v>
       </c>
       <c r="M6" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="N6">
-        <v>0.25383896237870601</v>
+        <v>5.6196606453970052E-2</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3050,10 +3050,10 @@
         <v>171</v>
       </c>
       <c r="M7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N7">
-        <v>5.6196606453970052E-2</v>
+        <v>0.1215100097787425</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3085,10 +3085,10 @@
         <v>171</v>
       </c>
       <c r="M8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N8">
-        <v>6.1341729440462497E-2</v>
+        <v>0.25383896237870596</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="N9">
-        <v>0.64374644043026452</v>
+        <v>6.134172944046249E-2</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000D6DF5-064C-4B0B-8190-C36DF1AAADE8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DCB29F-F56B-446F-90B3-80C63C572DF0}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 09:37
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63116DB-65DB-4EAD-B876-8606EC3A4D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4498060-C76A-4D43-9B20-80602470B98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S4aH2,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S1aH6,S3b0330h11,S6d1221h11,S3b0330h13,S6aH5,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S6d1221h08,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH2,S3b0330h07,S3b0330h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3aH3,S3b0330h15,S6d1221h13</t>
-  </si>
-  <si>
-    <t>S2aH1,S5aH8,S3aH1,S4c0615h24,S6d1221h01,S2aH8,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S1aH1,S3b0330h04,S3b0330h01,S3b0330h03,S4c0615h05,S4aH1,S4c0615h04,S6aH1,S6d1221h21,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h20,S4c0615h01,S6d1221h03,S3b0330h19,S4c0615h20,S3b0330h06,S3b0330h21</t>
+    <t>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S6d1221h08,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3aH2,S3b0330h07,S3b0330h17,S3b0330h14,S6aH7,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S4aH2,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3b0330h13,S6aH5,S1aH6,S3b0330h11,S6d1221h11,S3aH3,S3b0330h15,S6d1221h13,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18</t>
+  </si>
+  <si>
+    <t>S3b0330h01,S3b0330h03,S4c0615h05,S1aH1,S3b0330h04,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S3b0330h05,S4c0615h21,S6d1221h06,S6d1221h21,S3b0330h19,S4c0615h20,S4aH1,S4c0615h04,S6aH1,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3aH1,S4c0615h24,S6d1221h01,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S2aH1,S5aH8,S2aH8,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h06,S3b0330h21,S3b0330h20,S4c0615h01,S6d1221h03</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S2aH1,S5aH8,S3aH1,S4c0615h24,S6d1221h01,S2aH8,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S1aH1,S3b0330h04,S3b0330h01,S3b0330h03,S4c0615h05,S4aH1,S4c0615h04,S6aH1,S6d1221h21,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h20,S4c0615h01,S6d1221h03,S3b0330h19,S4c0615h20,S3b0330h06,S3b0330h21</v>
+        <v>S3b0330h01,S3b0330h03,S4c0615h05,S1aH1,S3b0330h04,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S3b0330h05,S4c0615h21,S6d1221h06,S6d1221h21,S3b0330h19,S4c0615h20,S4aH1,S4c0615h04,S6aH1,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3aH1,S4c0615h24,S6d1221h01,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S2aH1,S5aH8,S2aH8,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h06,S3b0330h21,S3b0330h20,S4c0615h01,S6d1221h03</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S4aH2,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S1aH6,S3b0330h11,S6d1221h11,S3b0330h13,S6aH5,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S6d1221h08,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH2,S3b0330h07,S3b0330h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3aH3,S3b0330h15,S6d1221h13</v>
+        <v>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S6d1221h08,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3aH2,S3b0330h07,S3b0330h17,S3b0330h14,S6aH7,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S4aH2,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3b0330h13,S6aH5,S1aH6,S3b0330h11,S6d1221h11,S3aH3,S3b0330h15,S6d1221h13,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FF797E-EDA3-4AE5-B67D-71DAE26DAA37}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F824AEFB-8F0F-466B-831F-03FC0F383F56}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBD3115-5910-403B-A207-72C1AC0F67F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35FC7119-4AE8-43E8-8E36-1087B4521DC3}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2945,10 +2945,10 @@
         <v>171</v>
       </c>
       <c r="M4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="N4">
-        <v>0.64374644043026452</v>
+        <v>6.1341729440462497E-2</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="N5">
-        <v>6.3366251517854258E-2</v>
+        <v>0.64374644043026452</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3015,10 +3015,10 @@
         <v>171</v>
       </c>
       <c r="M6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N6">
-        <v>5.6196606453970052E-2</v>
+        <v>0.12151000977874252</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3050,10 +3050,10 @@
         <v>171</v>
       </c>
       <c r="M7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N7">
-        <v>0.1215100097787425</v>
+        <v>0.25383896237870601</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3085,10 +3085,10 @@
         <v>171</v>
       </c>
       <c r="M8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="N8">
-        <v>0.25383896237870596</v>
+        <v>6.3366251517854258E-2</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="N9">
-        <v>6.134172944046249E-2</v>
+        <v>5.6196606453970052E-2</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DCB29F-F56B-446F-90B3-80C63C572DF0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E75B1554-3617-40CC-BFAB-FFA0FAC0092B}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 13:48
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446151B8-6234-45CE-8473-27E76D09B0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED444D6-7451-4304-BD06-A1E3D737EDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S4aH2,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S6d1221h08,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH6,S3b0330h11,S6d1221h11,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S3aH2,S3b0330h07,S3b0330h17,S3b0330h14,S6aH7,S3b0330h13,S6aH5,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH3,S3b0330h15,S6d1221h13</t>
-  </si>
-  <si>
-    <t>S2aH1,S5aH8,S3b0330h05,S4c0615h21,S6d1221h06,S6d1221h21,S3b0330h01,S3b0330h03,S4c0615h05,S1aH1,S3b0330h04,S2aH8,S3b0330h19,S4c0615h20,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S4aH1,S4c0615h04,S6aH1,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3aH1,S4c0615h24,S6d1221h01,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3b0330h20,S4c0615h01,S6d1221h03,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3b0330h06,S3b0330h21</t>
+    <t>S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3b0330h14,S6aH7,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S1aH6,S3b0330h11,S6d1221h11,S3aH3,S3b0330h15,S6d1221h13,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH2,S3b0330h07,S3b0330h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S6d1221h08,S4aH2,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h13,S6aH5</t>
+  </si>
+  <si>
+    <t>S3b0330h05,S4c0615h21,S6d1221h06,S6d1221h21,S3aH1,S4c0615h24,S6d1221h01,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h06,S3b0330h21,S3b0330h20,S4c0615h01,S6d1221h03,S2aH8,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S1aH1,S3b0330h04,S2aH1,S5aH8,S3b0330h19,S4c0615h20,S4aH1,S4c0615h04,S6aH1,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S2aH1,S5aH8,S3b0330h05,S4c0615h21,S6d1221h06,S6d1221h21,S3b0330h01,S3b0330h03,S4c0615h05,S1aH1,S3b0330h04,S2aH8,S3b0330h19,S4c0615h20,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S4aH1,S4c0615h04,S6aH1,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3aH1,S4c0615h24,S6d1221h01,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3b0330h20,S4c0615h01,S6d1221h03,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3b0330h06,S3b0330h21</v>
+        <v>S3b0330h05,S4c0615h21,S6d1221h06,S6d1221h21,S3aH1,S4c0615h24,S6d1221h01,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h06,S3b0330h21,S3b0330h20,S4c0615h01,S6d1221h03,S2aH8,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S1aH1,S3b0330h04,S2aH1,S5aH8,S3b0330h19,S4c0615h20,S4aH1,S4c0615h04,S6aH1,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S4aH2,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S6d1221h08,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH6,S3b0330h11,S6d1221h11,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S3aH2,S3b0330h07,S3b0330h17,S3b0330h14,S6aH7,S3b0330h13,S6aH5,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH3,S3b0330h15,S6d1221h13</v>
+        <v>S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3b0330h14,S6aH7,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S1aH6,S3b0330h11,S6d1221h11,S3aH3,S3b0330h15,S6d1221h13,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH2,S3b0330h07,S3b0330h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S6d1221h08,S4aH2,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h13,S6aH5</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CFF77A-7127-4EFE-B80A-8C9812EFF66F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5677513-F319-4DFA-A2B5-4FEFCCCADAAF}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22FCF02-091C-469A-AC6A-0CE4C6B44199}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5679591E-1774-41D9-BED0-E9D3F6EBD94C}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2945,10 +2945,10 @@
         <v>171</v>
       </c>
       <c r="M4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N4">
-        <v>0.12151000977874252</v>
+        <v>0.25383896237870601</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="N5">
-        <v>0.64374644043026452</v>
+        <v>0.12151000977874254</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3018,7 +3018,7 @@
         <v>87</v>
       </c>
       <c r="N6">
-        <v>5.6196606453970052E-2</v>
+        <v>5.6196606453970073E-2</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3053,7 +3053,7 @@
         <v>76</v>
       </c>
       <c r="N7">
-        <v>6.3366251517854258E-2</v>
+        <v>6.3366251517854272E-2</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3085,10 +3085,10 @@
         <v>171</v>
       </c>
       <c r="M8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N8">
-        <v>0.25383896237870596</v>
+        <v>6.1341729440462518E-2</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="N9">
-        <v>6.1341729440462497E-2</v>
+        <v>0.64374644043026474</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF841203-0C78-4287-A691-DE7C9ADB5424}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796B0839-842B-4B70-8ABE-1BF145DF47DA}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 14:10
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED444D6-7451-4304-BD06-A1E3D737EDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FD8E2F-ABD9-4B14-A47B-3A8326BCB92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3b0330h14,S6aH7,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S1aH6,S3b0330h11,S6d1221h11,S3aH3,S3b0330h15,S6d1221h13,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH2,S3b0330h07,S3b0330h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S6d1221h08,S4aH2,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h13,S6aH5</t>
-  </si>
-  <si>
-    <t>S3b0330h05,S4c0615h21,S6d1221h06,S6d1221h21,S3aH1,S4c0615h24,S6d1221h01,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h06,S3b0330h21,S3b0330h20,S4c0615h01,S6d1221h03,S2aH8,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S1aH1,S3b0330h04,S2aH1,S5aH8,S3b0330h19,S4c0615h20,S4aH1,S4c0615h04,S6aH1,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02</t>
+    <t>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S6d1221h08,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3aH2,S3b0330h07,S3b0330h17,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3b0330h13,S6aH5,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3aH3,S3b0330h15,S6d1221h13,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S1aH6,S3b0330h11,S6d1221h11,S4aH2</t>
+  </si>
+  <si>
+    <t>S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h20,S4c0615h01,S6d1221h03,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S1aH1,S3b0330h04,S6d1221h21,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h19,S4c0615h20,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3aH1,S4c0615h24,S6d1221h01,S2aH8,S3b0330h06,S3b0330h21,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4aH1,S4c0615h04,S6aH1,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S2aH1,S5aH8</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S3b0330h05,S4c0615h21,S6d1221h06,S6d1221h21,S3aH1,S4c0615h24,S6d1221h01,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3b0330h06,S3b0330h21,S3b0330h20,S4c0615h01,S6d1221h03,S2aH8,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S1aH1,S3b0330h04,S2aH1,S5aH8,S3b0330h19,S4c0615h20,S4aH1,S4c0615h04,S6aH1,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02</v>
+        <v>S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h20,S4c0615h01,S6d1221h03,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S1aH1,S3b0330h04,S6d1221h21,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h19,S4c0615h20,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3aH1,S4c0615h24,S6d1221h01,S2aH8,S3b0330h06,S3b0330h21,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4aH1,S4c0615h04,S6aH1,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S2aH1,S5aH8</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3b0330h14,S6aH7,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S1aH6,S3b0330h11,S6d1221h11,S3aH3,S3b0330h15,S6d1221h13,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH2,S3b0330h07,S3b0330h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S6d1221h08,S4aH2,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h13,S6aH5</v>
+        <v>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S6d1221h08,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3aH2,S3b0330h07,S3b0330h17,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3b0330h13,S6aH5,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3aH3,S3b0330h15,S6d1221h13,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S1aH6,S3b0330h11,S6d1221h11,S4aH2</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5677513-F319-4DFA-A2B5-4FEFCCCADAAF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D7FEFF-0D6D-4761-98F1-B3E0D28523F6}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5679591E-1774-41D9-BED0-E9D3F6EBD94C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31320041-05FE-4536-86B4-2E2D1985A1A7}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="N5">
-        <v>0.12151000977874254</v>
+        <v>0.64374644043026474</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3015,10 +3015,10 @@
         <v>171</v>
       </c>
       <c r="M6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N6">
-        <v>5.6196606453970073E-2</v>
+        <v>0.12151000977874253</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3050,10 +3050,10 @@
         <v>171</v>
       </c>
       <c r="M7" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N7">
-        <v>6.3366251517854272E-2</v>
+        <v>6.1341729440462511E-2</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3085,10 +3085,10 @@
         <v>171</v>
       </c>
       <c r="M8" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="N8">
-        <v>6.1341729440462518E-2</v>
+        <v>5.6196606453970059E-2</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="N9">
-        <v>0.64374644043026474</v>
+        <v>6.3366251517854272E-2</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796B0839-842B-4B70-8ABE-1BF145DF47DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5563167-B79E-4CC5-BD7A-896D3A114663}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 14:19
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FD8E2F-ABD9-4B14-A47B-3A8326BCB92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C2ED3E-2A50-42E2-BBE3-A1268F9DD0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S6d1221h08,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3aH2,S3b0330h07,S3b0330h17,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3b0330h13,S6aH5,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3aH3,S3b0330h15,S6d1221h13,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S1aH6,S3b0330h11,S6d1221h11,S4aH2</t>
-  </si>
-  <si>
-    <t>S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h20,S4c0615h01,S6d1221h03,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S1aH1,S3b0330h04,S6d1221h21,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h19,S4c0615h20,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3aH1,S4c0615h24,S6d1221h01,S2aH8,S3b0330h06,S3b0330h21,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4aH1,S4c0615h04,S6aH1,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S2aH1,S5aH8</t>
+    <t>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3b0330h13,S6aH5,S6d1221h08,S3b0330h14,S6aH7,S4aH2,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3aH3,S3b0330h15,S6d1221h13,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3aH2,S3b0330h07,S3b0330h17,S1aH6,S3b0330h11,S6d1221h11,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18</t>
+  </si>
+  <si>
+    <t>S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S1aH1,S3b0330h04,S3aH1,S4c0615h24,S6d1221h01,S2aH1,S5aH8,S4aH1,S4c0615h04,S6aH1,S3b0330h06,S3b0330h21,S6d1221h21,S3b0330h19,S4c0615h20,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S2aH8,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h20,S4c0615h01,S6d1221h03</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h20,S4c0615h01,S6d1221h03,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S1aH1,S3b0330h04,S6d1221h21,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h19,S4c0615h20,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3aH1,S4c0615h24,S6d1221h01,S2aH8,S3b0330h06,S3b0330h21,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4aH1,S4c0615h04,S6aH1,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S2aH1,S5aH8</v>
+        <v>S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S1aH1,S3b0330h04,S3aH1,S4c0615h24,S6d1221h01,S2aH1,S5aH8,S4aH1,S4c0615h04,S6aH1,S3b0330h06,S3b0330h21,S6d1221h21,S3b0330h19,S4c0615h20,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S2aH8,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h20,S4c0615h01,S6d1221h03</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S6d1221h08,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3aH2,S3b0330h07,S3b0330h17,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3b0330h13,S6aH5,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3aH3,S3b0330h15,S6d1221h13,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S1aH6,S3b0330h11,S6d1221h11,S4aH2</v>
+        <v>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3b0330h13,S6aH5,S6d1221h08,S3b0330h14,S6aH7,S4aH2,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3aH3,S3b0330h15,S6d1221h13,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3aH2,S3b0330h07,S3b0330h17,S1aH6,S3b0330h11,S6d1221h11,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D7FEFF-0D6D-4761-98F1-B3E0D28523F6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D135C8-58F1-43E7-9941-7B548A35E76E}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31320041-05FE-4536-86B4-2E2D1985A1A7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B749AE1-AA45-4145-8A87-11430A802664}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2945,10 +2945,10 @@
         <v>171</v>
       </c>
       <c r="M4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N4">
-        <v>0.25383896237870601</v>
+        <v>0.1215100097787425</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N5">
-        <v>0.64374644043026474</v>
+        <v>0.2538389623787059</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3015,10 +3015,10 @@
         <v>171</v>
       </c>
       <c r="M6" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="N6">
-        <v>0.12151000977874253</v>
+        <v>6.3366251517854258E-2</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3050,10 +3050,10 @@
         <v>171</v>
       </c>
       <c r="M7" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="N7">
-        <v>6.1341729440462511E-2</v>
+        <v>0.64374644043026441</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3085,10 +3085,10 @@
         <v>171</v>
       </c>
       <c r="M8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="N8">
-        <v>5.6196606453970059E-2</v>
+        <v>6.134172944046249E-2</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="N9">
-        <v>6.3366251517854272E-2</v>
+        <v>5.6196606453970052E-2</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5563167-B79E-4CC5-BD7A-896D3A114663}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24DFDD72-FE37-49E4-8104-CF7DBA53BDDA}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 14:28
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C2ED3E-2A50-42E2-BBE3-A1268F9DD0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0839EC3-E8E4-4BBB-B62D-7308EA073F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3b0330h13,S6aH5,S6d1221h08,S3b0330h14,S6aH7,S4aH2,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3aH3,S3b0330h15,S6d1221h13,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3aH2,S3b0330h07,S3b0330h17,S1aH6,S3b0330h11,S6d1221h11,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18</t>
-  </si>
-  <si>
-    <t>S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S1aH1,S3b0330h04,S3aH1,S4c0615h24,S6d1221h01,S2aH1,S5aH8,S4aH1,S4c0615h04,S6aH1,S3b0330h06,S3b0330h21,S6d1221h21,S3b0330h19,S4c0615h20,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S2aH8,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h20,S4c0615h01,S6d1221h03</t>
+    <t>S1aH6,S3b0330h11,S6d1221h11,S3b0330h14,S6aH7,S3aH3,S3b0330h15,S6d1221h13,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3b0330h13,S6aH5,S4aH2,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S6d1221h08,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3aH2,S3b0330h07,S3b0330h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15</t>
+  </si>
+  <si>
+    <t>S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3aH1,S4c0615h24,S6d1221h01,S3b0330h06,S3b0330h21,S6d1221h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S2aH1,S5aH8,S4aH1,S4c0615h04,S6aH1,S1aH1,S3b0330h04,S3b0330h19,S4c0615h20,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h20,S4c0615h01,S6d1221h03,S2aH8</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S1aH1,S3b0330h04,S3aH1,S4c0615h24,S6d1221h01,S2aH1,S5aH8,S4aH1,S4c0615h04,S6aH1,S3b0330h06,S3b0330h21,S6d1221h21,S3b0330h19,S4c0615h20,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S2aH8,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h20,S4c0615h01,S6d1221h03</v>
+        <v>S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3aH1,S4c0615h24,S6d1221h01,S3b0330h06,S3b0330h21,S6d1221h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S2aH1,S5aH8,S4aH1,S4c0615h04,S6aH1,S1aH1,S3b0330h04,S3b0330h19,S4c0615h20,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h20,S4c0615h01,S6d1221h03,S2aH8</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3b0330h13,S6aH5,S6d1221h08,S3b0330h14,S6aH7,S4aH2,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3aH3,S3b0330h15,S6d1221h13,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3aH2,S3b0330h07,S3b0330h17,S1aH6,S3b0330h11,S6d1221h11,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18</v>
+        <v>S1aH6,S3b0330h11,S6d1221h11,S3b0330h14,S6aH7,S3aH3,S3b0330h15,S6d1221h13,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3b0330h13,S6aH5,S4aH2,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S6d1221h08,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3aH2,S3b0330h07,S3b0330h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D135C8-58F1-43E7-9941-7B548A35E76E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8500AA-56D7-46A7-BAE1-1CEABAF3C99B}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B749AE1-AA45-4145-8A87-11430A802664}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E095EB0-59B0-4322-9B12-1509B01E9763}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2945,10 +2945,10 @@
         <v>171</v>
       </c>
       <c r="M4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="N4">
-        <v>0.1215100097787425</v>
+        <v>6.3366251517854258E-2</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -3015,10 +3015,10 @@
         <v>171</v>
       </c>
       <c r="M6" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="N6">
-        <v>6.3366251517854258E-2</v>
+        <v>0.1215100097787425</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3053,7 +3053,7 @@
         <v>88</v>
       </c>
       <c r="N7">
-        <v>0.64374644043026441</v>
+        <v>0.64374644043026452</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3085,10 +3085,10 @@
         <v>171</v>
       </c>
       <c r="M8" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="N8">
-        <v>6.134172944046249E-2</v>
+        <v>5.6196606453970052E-2</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="N9">
-        <v>5.6196606453970052E-2</v>
+        <v>6.134172944046249E-2</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24DFDD72-FE37-49E4-8104-CF7DBA53BDDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8376AFA-B70C-4454-898E-7F28F925E148}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 15:47
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0839EC3-E8E4-4BBB-B62D-7308EA073F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E67FFFF-3FBF-47F4-8284-E5A25CF09114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S1aH6,S3b0330h11,S6d1221h11,S3b0330h14,S6aH7,S3aH3,S3b0330h15,S6d1221h13,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3b0330h13,S6aH5,S4aH2,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S6d1221h08,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3aH2,S3b0330h07,S3b0330h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15</t>
-  </si>
-  <si>
-    <t>S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3aH1,S4c0615h24,S6d1221h01,S3b0330h06,S3b0330h21,S6d1221h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S2aH1,S5aH8,S4aH1,S4c0615h04,S6aH1,S1aH1,S3b0330h04,S3b0330h19,S4c0615h20,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h20,S4c0615h01,S6d1221h03,S2aH8</t>
+    <t>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S1aH6,S3b0330h11,S6d1221h11,S6d1221h08,S4aH2,S3aH3,S3b0330h15,S6d1221h13,S3b0330h13,S6aH5,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH2,S3b0330h07,S3b0330h17,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15</t>
+  </si>
+  <si>
+    <t>S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S1aH1,S3b0330h04,S2aH1,S5aH8,S3b0330h06,S3b0330h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3b0330h20,S4c0615h01,S6d1221h03,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S3b0330h19,S4c0615h20,S4aH1,S4c0615h04,S6aH1,S3b0330h05,S4c0615h21,S6d1221h06,S6d1221h21,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3aH1,S4c0615h24,S6d1221h01,S2aH8</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S3aH1,S4c0615h24,S6d1221h01,S3b0330h06,S3b0330h21,S6d1221h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S2aH1,S5aH8,S4aH1,S4c0615h04,S6aH1,S1aH1,S3b0330h04,S3b0330h19,S4c0615h20,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3b0330h05,S4c0615h21,S6d1221h06,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h20,S4c0615h01,S6d1221h03,S2aH8</v>
+        <v>S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S1aH1,S3b0330h04,S2aH1,S5aH8,S3b0330h06,S3b0330h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3b0330h20,S4c0615h01,S6d1221h03,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S3b0330h19,S4c0615h20,S4aH1,S4c0615h04,S6aH1,S3b0330h05,S4c0615h21,S6d1221h06,S6d1221h21,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3aH1,S4c0615h24,S6d1221h01,S2aH8</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S1aH6,S3b0330h11,S6d1221h11,S3b0330h14,S6aH7,S3aH3,S3b0330h15,S6d1221h13,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S3b0330h13,S6aH5,S4aH2,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S6d1221h08,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S3aH2,S3b0330h07,S3b0330h17,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15</v>
+        <v>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S1aH6,S3b0330h11,S6d1221h11,S6d1221h08,S4aH2,S3aH3,S3b0330h15,S6d1221h13,S3b0330h13,S6aH5,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH2,S3b0330h07,S3b0330h17,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8500AA-56D7-46A7-BAE1-1CEABAF3C99B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{801F26C1-20FD-4D89-9088-DACFC141112B}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E095EB0-59B0-4322-9B12-1509B01E9763}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7BD855-C93F-4957-9AAC-8943EB39805D}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2948,7 +2948,7 @@
         <v>76</v>
       </c>
       <c r="N4">
-        <v>6.3366251517854258E-2</v>
+        <v>6.3366251517854272E-2</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N5">
-        <v>0.2538389623787059</v>
+        <v>0.12151000977874253</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3015,10 +3015,10 @@
         <v>171</v>
       </c>
       <c r="M6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="N6">
-        <v>0.1215100097787425</v>
+        <v>6.1341729440462511E-2</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3053,7 +3053,7 @@
         <v>88</v>
       </c>
       <c r="N7">
-        <v>0.64374644043026452</v>
+        <v>0.64374644043026463</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3088,7 +3088,7 @@
         <v>87</v>
       </c>
       <c r="N8">
-        <v>5.6196606453970052E-2</v>
+        <v>5.6196606453970059E-2</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N9">
-        <v>6.134172944046249E-2</v>
+        <v>0.25383896237870601</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8376AFA-B70C-4454-898E-7F28F925E148}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F38888-336F-4C22-A693-6F33D897C504}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 16:39
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_IND/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E67FFFF-3FBF-47F4-8284-E5A25CF09114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1174B113-5BA9-40BE-BE59-BE68B049D01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" firstSheet="3" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
   <sheets>
     <sheet name="ev_charging_uc" sheetId="9" r:id="rId1"/>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S1aH6,S3b0330h11,S6d1221h11,S6d1221h08,S4aH2,S3aH3,S3b0330h15,S6d1221h13,S3b0330h13,S6aH5,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH2,S3b0330h07,S3b0330h17,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15</t>
-  </si>
-  <si>
-    <t>S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S1aH1,S3b0330h04,S2aH1,S5aH8,S3b0330h06,S3b0330h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3b0330h20,S4c0615h01,S6d1221h03,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S3b0330h19,S4c0615h20,S4aH1,S4c0615h04,S6aH1,S3b0330h05,S4c0615h21,S6d1221h06,S6d1221h21,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3aH1,S4c0615h24,S6d1221h01,S2aH8</t>
+    <t>S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3aH3,S3b0330h15,S6d1221h13,S6d1221h08,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h14,S6aH7,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4aH2,S1aH6,S3b0330h11,S6d1221h11,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S3b0330h13,S6aH5,S3aH2,S3b0330h07,S3b0330h17</t>
+  </si>
+  <si>
+    <t>S2aH8,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h06,S3b0330h21,S1aH1,S3b0330h04,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S6d1221h21,S3b0330h19,S4c0615h20,S3b0330h20,S4c0615h01,S6d1221h03,S4aH1,S4c0615h04,S6aH1,S3aH1,S4c0615h24,S6d1221h01,S3b0330h05,S4c0615h21,S6d1221h06,S2aH1,S5aH8,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S1aH1,S3b0330h04,S2aH1,S5aH8,S3b0330h06,S3b0330h21,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3b0330h20,S4c0615h01,S6d1221h03,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S3b0330h19,S4c0615h20,S4aH1,S4c0615h04,S6aH1,S3b0330h05,S4c0615h21,S6d1221h06,S6d1221h21,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05,S3aH1,S4c0615h24,S6d1221h01,S2aH8</v>
+        <v>S2aH8,S3b0330h01,S3b0330h03,S4c0615h05,S3b0330h06,S3b0330h21,S1aH1,S3b0330h04,S4c0615h06,S6d1221h04,S6d1221h19,S6d1221h24,S6d1221h21,S3b0330h19,S4c0615h20,S3b0330h20,S4c0615h01,S6d1221h03,S4aH1,S4c0615h04,S6aH1,S3aH1,S4c0615h24,S6d1221h01,S3b0330h05,S4c0615h21,S6d1221h06,S2aH1,S5aH8,S3b0330h22,S4c0615h03,S6aH8,S6d1221h20,S6d1221h22,S1aH8,S3b0330h02,S4c0615h23,S5aH1,S6d1221h23,S3b0330h23,S3b0330h24,S4aH8,S4c0615h02,S3aH8,S4c0615h19,S4c0615h22,S6d1221h02,S6d1221h05</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S1aH6,S3b0330h11,S6d1221h11,S6d1221h08,S4aH2,S3aH3,S3b0330h15,S6d1221h13,S3b0330h13,S6aH5,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S3aH2,S3b0330h07,S3b0330h17,S3b0330h14,S6aH7,S3aH7,S3b0330h18,S4c0615h12,S6d1221h15</v>
+        <v>S3aH7,S3b0330h18,S4c0615h12,S6d1221h15,S1aH2,S1aH7,S2aH3,S3aH6,S3b0330h08,S4aH7,S4c0615h08,S5aH6,S5aH7,S6aH6,S3aH3,S3b0330h15,S6d1221h13,S6d1221h08,S2aH7,S3aH4,S3b0330h10,S3b0330h16,S4aH3,S4aH4,S4c0615h17,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S1aH3,S4c0615h09,S6d1221h07,S6d1221h14,S6d1221h16,S4c0615h10,S4c0615h13,S4c0615h18,S5aH4,S6aH3,S6aH4,S6d1221h09,S6d1221h12,S6d1221h18,S1aH4,S2aH2,S3b0330h12,S4aH6,S4c0615h16,S6d1221h17,S3b0330h14,S6aH7,S3b0330h09,S4aH5,S4c0615h07,S4c0615h14,S6d1221h10,S4aH2,S1aH6,S3b0330h11,S6d1221h11,S2aH6,S3aH5,S4c0615h11,S4c0615h15,S5aH3,S3b0330h13,S6aH5,S3aH2,S3b0330h07,S3b0330h17</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{801F26C1-20FD-4D89-9088-DACFC141112B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54292F04-0CC2-4364-802F-4E1E546BCA64}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7BD855-C93F-4957-9AAC-8943EB39805D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50C1C8A-4804-4A99-ABD6-19C5FAAF501D}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2945,10 +2945,10 @@
         <v>171</v>
       </c>
       <c r="M4" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="N4">
-        <v>6.3366251517854272E-2</v>
+        <v>0.64374644043026463</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="N5">
-        <v>0.12151000977874253</v>
+        <v>5.6196606453970059E-2</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3050,10 +3050,10 @@
         <v>171</v>
       </c>
       <c r="M7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="N7">
-        <v>0.64374644043026463</v>
+        <v>0.12151000977874253</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3085,10 +3085,10 @@
         <v>171</v>
       </c>
       <c r="M8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="N8">
-        <v>5.6196606453970059E-2</v>
+        <v>0.25383896237870601</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="N9">
-        <v>0.25383896237870601</v>
+        <v>6.3366251517854272E-2</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F38888-336F-4C22-A693-6F33D897C504}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A1E7D3-E1AE-4452-9641-482D43957B7B}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>